<commit_message>
small format change for graph
</commit_message>
<xml_diff>
--- a/dataAnalysis/test results qs.xlsx
+++ b/dataAnalysis/test results qs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITU\Kand\2.Semester\AlgorithmDesignProject\quadsketch\dataAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A316BCF-031A-466D-B401-FC46DA0EF1D8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB372E20-0C02-42D2-8C06-1500BC2BB6D4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,10 +600,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -753,10 +751,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1206,10 +1202,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2805,7 +2799,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -10468,7 +10462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C5DF786-259B-45AA-8FC1-8E62C49324A3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>

</xml_diff>